<commit_message>
OpenMP built-in, more results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="OpenMP" sheetId="1" r:id="rId1"/>
     <sheet name="MPI" sheetId="2" r:id="rId2"/>
     <sheet name="Combined" sheetId="3" r:id="rId3"/>
-    <sheet name="MPI-Combined" sheetId="4" r:id="rId4"/>
+    <sheet name="MPI-Combined-8" sheetId="4" r:id="rId4"/>
+    <sheet name="MPI-Combined-6" sheetId="5" r:id="rId5"/>
+    <sheet name="MPI-Combined-2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Counter barrier with sense reversal</t>
   </si>
@@ -48,6 +50,9 @@
   <si>
     <t>Combined barrier</t>
   </si>
+  <si>
+    <t>Built-in barrier</t>
+  </si>
 </sst>
 </file>
 
@@ -55,9 +60,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000E+00"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +81,16 @@
       <color rgb="FF500050"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF500050"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF222222"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,12 +113,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -204,7 +221,7 @@
             <c:v>Counter barrier</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="15875" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -356,7 +373,7 @@
             <c:v>Tournament barrier</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="15875" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -482,11 +499,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-222462688"/>
-        <c:axId val="-222455072"/>
+        <c:axId val="1838205424"/>
+        <c:axId val="2108369584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-222462688"/>
+        <c:axId val="1838205424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -615,7 +632,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-222455072"/>
+        <c:crossAx val="2108369584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -623,7 +640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-222455072"/>
+        <c:axId val="2108369584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -738,7 +755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-222462688"/>
+        <c:crossAx val="1838205424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -868,7 +885,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> barriers</a:t>
+              <a:t> Barriers</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -927,7 +944,7 @@
           <c:spPr>
             <a:ln w="15875" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -942,7 +959,7 @@
               </a:solidFill>
               <a:ln w="15875">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -1111,8 +1128,9 @@
           <c:spPr>
             <a:ln w="15875" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1126,7 +1144,150 @@
               </a:solidFill>
               <a:ln w="15875">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>MPI!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.0423710000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1859500000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2033860000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4032210000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3941460000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.7104720000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5859690000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.8011800000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.7596980000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.9676310000000008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.7760420000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MPI!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Built-in barrier</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -1194,42 +1355,42 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>MPI!$C$2:$C$12</c:f>
+              <c:f>MPI!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.0423710000000002</c:v>
+                  <c:v>1.925794</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1859500000000001</c:v>
+                  <c:v>4.2291400000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2033860000000001</c:v>
+                  <c:v>4.0923610000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.4032210000000003</c:v>
+                  <c:v>6.2710140000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.3941460000000001</c:v>
+                  <c:v>6.3702759999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.7104720000000002</c:v>
+                  <c:v>6.6857810000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5859690000000004</c:v>
+                  <c:v>6.3140390000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.8011800000000004</c:v>
+                  <c:v>8.6748820000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.7596980000000002</c:v>
+                  <c:v>8.6631529999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.9676310000000008</c:v>
+                  <c:v>8.9893239999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.7760420000000003</c:v>
+                  <c:v>9.1274239999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1246,11 +1407,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-154054096"/>
-        <c:axId val="-154055728"/>
+        <c:axId val="2108360336"/>
+        <c:axId val="2108360880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-154054096"/>
+        <c:axId val="2108360336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1384,7 +1545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-154055728"/>
+        <c:crossAx val="2108360880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1392,7 +1553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-154055728"/>
+        <c:axId val="2108360880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,7 +1665,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-154054096"/>
+        <c:crossAx val="2108360336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1681,7 +1842,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'MPI-Combined'!$B$1</c:f>
+              <c:f>'MPI-Combined-8'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1776,7 +1937,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'MPI-Combined'!$A$2:$A$8</c:f>
+              <c:f>'MPI-Combined-8'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1806,7 +1967,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'MPI-Combined'!$B$2:$B$8</c:f>
+              <c:f>'MPI-Combined-8'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1846,11 +2007,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-91726688"/>
-        <c:axId val="-91726144"/>
+        <c:axId val="2108357072"/>
+        <c:axId val="2108371760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-91726688"/>
+        <c:axId val="2108357072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1984,7 +2145,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-91726144"/>
+        <c:crossAx val="2108371760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1992,7 +2153,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-91726144"/>
+        <c:axId val="2108371760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2105,7 +2266,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-91726688"/>
+        <c:crossAx val="2108357072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2127,6 +2288,1274 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>MPI</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Combined (6 nodes)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MPI-Combined-6'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dissemination-MPI barrier</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'MPI-Combined-6'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9.5638020000000008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.925146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.840733999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.687512999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.956931000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.125209000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.667594000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2116381632"/>
+        <c:axId val="2116382720"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'MPI-Combined-6'!$A$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Number of processes per node</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="15875" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="4"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:ln w="15875">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="t"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:layout/>
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'MPI-Combined-6'!$B$2:$B$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.000</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>9.5638020000000008</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>11.925146</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>11.840733999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>13.687512999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>30.956931000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22.125209000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>28.667594000000001</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2116381632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of processes per node</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2116382720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2116382720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Avg.</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time per barrier (us)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2116381632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.8219837073679914E-2"/>
+          <c:y val="0.20294041994750656"/>
+          <c:w val="0.87122462817147861"/>
+          <c:h val="0.63966025080198308"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MPI-Combined-2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dissemination-MPI barrier</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'MPI-Combined-2'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'MPI-Combined-2'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.8005330000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3168230000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3316270000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0551849999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1975259999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1617189999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.3577459999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="148221776"/>
+        <c:axId val="148220688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="148221776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of processes per node</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="148220688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="148220688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Avg. time per barrier (us)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="148221776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2284,6 +3713,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
@@ -3387,6 +4896,1108 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4017,14 +6628,86 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4332,7 +7015,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4441,10 +7124,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4453,7 +7136,7 @@
     <col min="2" max="2" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4463,8 +7146,11 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4474,8 +7160,11 @@
       <c r="C2" s="3">
         <v>2.0423710000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="6">
+        <v>1.925794</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4485,8 +7174,11 @@
       <c r="C3" s="3">
         <v>4.1859500000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="6">
+        <v>4.2291400000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -4496,8 +7188,11 @@
       <c r="C4" s="3">
         <v>4.2033860000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="6">
+        <v>4.0923610000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -4507,8 +7202,11 @@
       <c r="C5" s="3">
         <v>6.4032210000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="6">
+        <v>6.2710140000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -4518,8 +7216,11 @@
       <c r="C6" s="3">
         <v>6.3941460000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="6">
+        <v>6.3702759999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -4529,8 +7230,11 @@
       <c r="C7" s="3">
         <v>6.7104720000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="6">
+        <v>6.6857810000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -4540,8 +7244,11 @@
       <c r="C8" s="3">
         <v>6.5859690000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="6">
+        <v>6.3140390000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -4551,8 +7258,11 @@
       <c r="C9" s="3">
         <v>8.8011800000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="6">
+        <v>8.6748820000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -4562,8 +7272,11 @@
       <c r="C10" s="3">
         <v>8.7596980000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="6">
+        <v>8.6631529999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -4573,8 +7286,11 @@
       <c r="C11" s="3">
         <v>8.9676310000000008</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="6">
+        <v>8.9893239999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -4583,6 +7299,9 @@
       </c>
       <c r="C12" s="3">
         <v>8.7760420000000003</v>
+      </c>
+      <c r="D12" s="6">
+        <v>9.1274239999999995</v>
       </c>
     </row>
   </sheetData>
@@ -4942,8 +7661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5023,4 +7742,171 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>9.5638020000000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6">
+        <v>11.925146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>11.840733999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6">
+        <v>13.687512999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6">
+        <v>30.956931000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6">
+        <v>22.125209000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <v>28.667594000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6">
+        <v>3.8005330000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6">
+        <v>5.3168230000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>5.3316270000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6">
+        <v>7.0551849999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6">
+        <v>7.1975259999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6">
+        <v>7.1617189999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <v>7.3577459999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Write-up and results updated
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="OpenMP" sheetId="1" r:id="rId1"/>
     <sheet name="MPI" sheetId="2" r:id="rId2"/>
     <sheet name="Combined" sheetId="3" r:id="rId3"/>
-    <sheet name="MPI-Combined-8" sheetId="4" r:id="rId4"/>
-    <sheet name="MPI-Combined-6" sheetId="5" r:id="rId5"/>
-    <sheet name="MPI-Combined-2" sheetId="6" r:id="rId6"/>
+    <sheet name="MPI-Combined-2" sheetId="6" r:id="rId4"/>
+    <sheet name="MPI-Combined-8" sheetId="4" r:id="rId5"/>
+    <sheet name="MPI-Combined-6" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -113,12 +113,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -1791,11 +1793,1831 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Combined barrier</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>2 nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Combined!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Combined!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.5645129999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7893629999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1777510000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.360789</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.553741</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7077049999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8272200000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3 nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Combined!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Combined!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.8639210000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0483700000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5517719999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8512729999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9618609999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0649769999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.2933190000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>4 nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Combined!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Combined!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.9122070000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.044009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5310730000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5546959999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9610989999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0893290000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3211529999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>5 nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Combined!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Combined!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.3287810000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.395562</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0635739999999991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0994499999999992</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5373040000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4698869999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.8652390000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>6 nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Combined!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Combined!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.4095399999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2294580000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7876989999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.9255069999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4796469999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4200769999999991</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.6715110000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>7 nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Combined!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Combined!$G$2:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.594004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0038879999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9424739999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3210010000000008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.8717740000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6455330000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.9689910000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>8 nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Combined!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Combined!$H$2:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.6141629999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9141849999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9689610000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4969370000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6418309999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.737603</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0007699999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="59578304"/>
+        <c:axId val="59578848"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="59578304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of threads per node</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="59578848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="59578848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Avg.</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time per barrier (us)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="59578304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>MPI vs Combined Barrier (2 nodes)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.8219837073679914E-2"/>
+          <c:y val="0.20294041994750656"/>
+          <c:w val="0.87122462817147861"/>
+          <c:h val="0.63966025080198308"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MPI-Combined-2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dissemination-MPI barrier</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'MPI-Combined-2'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'MPI-Combined-2'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.8005330000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3168230000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3316270000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0551849999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1975259999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1617189999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.3577459999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MPI-Combined-2'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Combined barrier</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'MPI-Combined-2'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.5645129999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7893629999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1777510000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.360789</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.553741</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7077049999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8272200000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="148221776"/>
+        <c:axId val="148220688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="148221776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of processes per node</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="148220688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="148220688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Avg. time per barrier (us)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="148221776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>MPI</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs Combined (8 nodes)</a:t>
+              <a:t> vs Combined Barrier (8 nodes)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1991,6 +3813,136 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>15.339098</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MPI-Combined-8'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Combined barrier</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'MPI-Combined-8'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.6141629999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9141849999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9689610000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4969370000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6418309999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.737603</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0007699999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2357,7 +4309,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3017,582 +4969,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="9.8219837073679914E-2"/>
-          <c:y val="0.20294041994750656"/>
-          <c:w val="0.87122462817147861"/>
-          <c:h val="0.63966025080198308"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'MPI-Combined-2'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Dissemination-MPI barrier</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="15875" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:ln w="15875">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>'MPI-Combined-2'!$A$2:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'MPI-Combined-2'!$B$2:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3.8005330000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.3168230000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.3316270000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.0551849999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.1975259999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.1617189999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.3577459999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="148221776"/>
-        <c:axId val="148220688"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="148221776"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                  <a:alpha val="54000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                  <a:alpha val="51000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Number</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of processes per node</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="148220688"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="148220688"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                  <a:alpha val="54000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Avg. time per barrier (us)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="148221776"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:pattFill prst="ltDnDiag">
-          <a:fgClr>
-            <a:schemeClr val="dk1">
-              <a:lumMod val="15000"/>
-              <a:lumOff val="85000"/>
-            </a:schemeClr>
-          </a:fgClr>
-          <a:bgClr>
-            <a:schemeClr val="lt1"/>
-          </a:bgClr>
-        </a:pattFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="lt1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3793,6 +5169,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
@@ -5998,6 +7414,557 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6622,6 +8589,76 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1661160</xdr:colOff>
       <xdr:row>8</xdr:row>
@@ -6653,7 +8690,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6674,41 +8711,6 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -7014,8 +9016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7160,7 +9162,7 @@
       <c r="C2" s="3">
         <v>2.0423710000000002</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="8">
         <v>1.925794</v>
       </c>
     </row>
@@ -7174,7 +9176,7 @@
       <c r="C3" s="3">
         <v>4.1859500000000001</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="8">
         <v>4.2291400000000001</v>
       </c>
     </row>
@@ -7188,7 +9190,7 @@
       <c r="C4" s="3">
         <v>4.2033860000000001</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="8">
         <v>4.0923610000000004</v>
       </c>
     </row>
@@ -7202,7 +9204,7 @@
       <c r="C5" s="3">
         <v>6.4032210000000003</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="8">
         <v>6.2710140000000001</v>
       </c>
     </row>
@@ -7216,7 +9218,7 @@
       <c r="C6" s="3">
         <v>6.3941460000000001</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="8">
         <v>6.3702759999999996</v>
       </c>
     </row>
@@ -7230,7 +9232,7 @@
       <c r="C7" s="3">
         <v>6.7104720000000002</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="8">
         <v>6.6857810000000004</v>
       </c>
     </row>
@@ -7244,7 +9246,7 @@
       <c r="C8" s="3">
         <v>6.5859690000000004</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="8">
         <v>6.3140390000000002</v>
       </c>
     </row>
@@ -7258,7 +9260,7 @@
       <c r="C9" s="3">
         <v>8.8011800000000004</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="8">
         <v>8.6748820000000002</v>
       </c>
     </row>
@@ -7272,7 +9274,7 @@
       <c r="C10" s="3">
         <v>8.7596980000000002</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="8">
         <v>8.6631529999999994</v>
       </c>
     </row>
@@ -7286,7 +9288,7 @@
       <c r="C11" s="3">
         <v>8.9676310000000008</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="8">
         <v>8.9893239999999999</v>
       </c>
     </row>
@@ -7300,7 +9302,7 @@
       <c r="C12" s="3">
         <v>8.7760420000000003</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="8">
         <v>9.1274239999999995</v>
       </c>
     </row>
@@ -7312,15 +9314,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -7342,318 +9344,198 @@
       <c r="G1">
         <v>7</v>
       </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>2.6312959999999999</v>
-      </c>
-      <c r="C2" s="2">
-        <v>4.9011979999999999</v>
-      </c>
-      <c r="D2" s="2">
-        <v>5.0346960000000003</v>
+      <c r="B2" s="6">
+        <v>2.5645129999999998</v>
+      </c>
+      <c r="C2" s="6">
+        <v>4.8639210000000004</v>
+      </c>
+      <c r="D2" s="6">
+        <v>4.9122070000000004</v>
+      </c>
+      <c r="E2" s="6">
+        <v>7.3287810000000002</v>
+      </c>
+      <c r="F2" s="6">
+        <v>7.4095399999999998</v>
+      </c>
+      <c r="G2" s="6">
+        <v>7.594004</v>
+      </c>
+      <c r="H2" s="6">
+        <v>7.6141629999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
-        <v>2.792764</v>
-      </c>
-      <c r="C3" s="2">
-        <v>5.1424960000000004</v>
-      </c>
-      <c r="D3" s="2">
-        <v>6.6922579999999998</v>
+      <c r="B3" s="6">
+        <v>2.7893629999999998</v>
+      </c>
+      <c r="C3" s="6">
+        <v>5.0483700000000002</v>
+      </c>
+      <c r="D3" s="6">
+        <v>5.044009</v>
+      </c>
+      <c r="E3" s="6">
+        <v>7.395562</v>
+      </c>
+      <c r="F3" s="6">
+        <v>7.2294580000000002</v>
+      </c>
+      <c r="G3" s="6">
+        <v>8.0038879999999999</v>
+      </c>
+      <c r="H3" s="6">
+        <v>7.9141849999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <v>3.2713220000000001</v>
-      </c>
-      <c r="C4" s="2">
-        <v>5.4861240000000002</v>
-      </c>
-      <c r="D4" s="2">
-        <v>5.6077459999999997</v>
+      <c r="B4" s="5">
+        <v>3.1777510000000002</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5.5517719999999997</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5.5310730000000001</v>
+      </c>
+      <c r="E4" s="6">
+        <v>8.0635739999999991</v>
+      </c>
+      <c r="F4" s="6">
+        <v>7.7876989999999999</v>
+      </c>
+      <c r="G4" s="6">
+        <v>7.9424739999999998</v>
+      </c>
+      <c r="H4" s="6">
+        <v>7.9689610000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
-        <v>3.5421499999999999</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5.9158819999999999</v>
-      </c>
-      <c r="D5" s="2">
-        <v>7.143332</v>
+      <c r="B5" s="6">
+        <v>3.360789</v>
+      </c>
+      <c r="C5" s="6">
+        <v>5.8512729999999999</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5.5546959999999999</v>
+      </c>
+      <c r="E5" s="6">
+        <v>8.0994499999999992</v>
+      </c>
+      <c r="F5" s="6">
+        <v>7.9255069999999996</v>
+      </c>
+      <c r="G5" s="6">
+        <v>8.3210010000000008</v>
+      </c>
+      <c r="H5" s="6">
+        <v>8.4969370000000009</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
-        <v>3.7378480000000001</v>
-      </c>
-      <c r="C6" s="2">
-        <v>6.2006079999999999</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5.8542940000000003</v>
+      <c r="B6" s="6">
+        <v>3.553741</v>
+      </c>
+      <c r="C6" s="6">
+        <v>5.9618609999999999</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5.9610989999999999</v>
+      </c>
+      <c r="E6" s="6">
+        <v>8.5373040000000007</v>
+      </c>
+      <c r="F6" s="5">
+        <v>8.4796469999999999</v>
+      </c>
+      <c r="G6" s="6">
+        <v>8.8717740000000003</v>
+      </c>
+      <c r="H6" s="6">
+        <v>8.6418309999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
-        <v>3.8112620000000001</v>
-      </c>
-      <c r="C7" s="2">
-        <v>6.0522980000000004</v>
-      </c>
-      <c r="D7" s="2">
-        <v>6.0555060000000003</v>
+      <c r="B7" s="6">
+        <v>3.7077049999999998</v>
+      </c>
+      <c r="C7" s="6">
+        <v>6.0649769999999998</v>
+      </c>
+      <c r="D7" s="6">
+        <v>6.0893290000000002</v>
+      </c>
+      <c r="E7" s="6">
+        <v>8.4698869999999999</v>
+      </c>
+      <c r="F7" s="6">
+        <v>8.4200769999999991</v>
+      </c>
+      <c r="G7" s="6">
+        <v>8.6455330000000004</v>
+      </c>
+      <c r="H7" s="6">
+        <v>8.737603</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
-        <v>3.891508</v>
-      </c>
-      <c r="C8" s="2">
-        <v>6.6661539999999997</v>
-      </c>
-      <c r="D8" s="2">
-        <v>6.3562320000000003</v>
+      <c r="B8" s="5">
+        <v>3.8272200000000001</v>
+      </c>
+      <c r="C8" s="6">
+        <v>6.2933190000000003</v>
+      </c>
+      <c r="D8" s="6">
+        <v>6.3211529999999998</v>
+      </c>
+      <c r="E8" s="6">
+        <v>8.8652390000000008</v>
+      </c>
+      <c r="F8" s="6">
+        <v>8.6715110000000006</v>
+      </c>
+      <c r="G8" s="6">
+        <v>8.9689910000000008</v>
+      </c>
+      <c r="H8" s="6">
+        <v>9.0007699999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2</v>
-      </c>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7662,14 +9544,10 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="27.88671875" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -7686,56 +9564,77 @@
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
-        <v>9.4331630000000004</v>
+      <c r="B2" s="8">
+        <v>3.8005330000000002</v>
+      </c>
+      <c r="C2" s="8">
+        <v>2.5645129999999998</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
-        <v>10.961081</v>
+      <c r="B3" s="8">
+        <v>5.3168230000000003</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2.7893629999999998</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
-        <v>11.141690000000001</v>
+      <c r="B4" s="8">
+        <v>5.3316270000000001</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3.1777510000000002</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
-        <v>13.102658</v>
+      <c r="B5" s="8">
+        <v>7.0551849999999998</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3.360789</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" s="3">
-        <v>13.752504999999999</v>
+      <c r="B6" s="8">
+        <v>7.1975259999999999</v>
+      </c>
+      <c r="C6" s="8">
+        <v>3.553741</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
-        <v>14.895047</v>
+      <c r="B7" s="8">
+        <v>7.1617189999999997</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3.7077049999999998</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
-        <v>15.339098</v>
+      <c r="B8" s="8">
+        <v>7.3577459999999997</v>
+      </c>
+      <c r="C8" s="7">
+        <v>3.8272200000000001</v>
       </c>
     </row>
   </sheetData>
@@ -7749,7 +9648,115 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+      <selection activeCell="C2" sqref="C2:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4">
+        <v>9.4331630000000004</v>
+      </c>
+      <c r="C2" s="8">
+        <v>7.6141629999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>10.961081</v>
+      </c>
+      <c r="C3" s="8">
+        <v>7.9141849999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>11.141690000000001</v>
+      </c>
+      <c r="C4" s="8">
+        <v>7.9689610000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>13.102658</v>
+      </c>
+      <c r="C5" s="8">
+        <v>8.4969370000000009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>13.752504999999999</v>
+      </c>
+      <c r="C6" s="8">
+        <v>8.6418309999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>14.895047</v>
+      </c>
+      <c r="C7" s="8">
+        <v>8.737603</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3">
+        <v>15.339098</v>
+      </c>
+      <c r="C8" s="8">
+        <v>9.0007699999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7769,7 +9776,7 @@
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="7">
         <v>9.5638020000000008</v>
       </c>
     </row>
@@ -7777,7 +9784,7 @@
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="8">
         <v>11.925146</v>
       </c>
     </row>
@@ -7785,7 +9792,7 @@
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="8">
         <v>11.840733999999999</v>
       </c>
     </row>
@@ -7793,7 +9800,7 @@
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="8">
         <v>13.687512999999999</v>
       </c>
     </row>
@@ -7801,7 +9808,7 @@
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="8">
         <v>30.956931000000001</v>
       </c>
     </row>
@@ -7809,7 +9816,7 @@
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="8">
         <v>22.125209000000002</v>
       </c>
     </row>
@@ -7817,7 +9824,7 @@
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="8">
         <v>28.667594000000001</v>
       </c>
     </row>
@@ -7826,87 +9833,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" s="6">
-        <v>3.8005330000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6">
-        <v>5.3168230000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6">
-        <v>5.3316270000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" s="6">
-        <v>7.0551849999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6">
-        <v>7.1975259999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6">
-        <v>7.1617189999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" s="6">
-        <v>7.3577459999999997</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>